<commit_message>
Disabled POST , enabled PUT (upsert) operation, updated utility
</commit_message>
<xml_diff>
--- a/customer-secure-api/utility/Calyx20250804.xlsx
+++ b/customer-secure-api/utility/Calyx20250804.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bajajfam/RS-dazpak/C-dazpak/customer-secure-api/utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4152FB-C897-8C49-9B77-2973CC5A6E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B016B1-730C-E145-94CA-2E799AE5D3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20520" yWindow="4100" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>Calyx20250804</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Plant</t>
   </si>
@@ -119,17 +116,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -278,17 +269,17 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -303,7 +294,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -320,9 +311,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1454,10 +1442,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1487,160 +1475,158 @@
     <col min="23" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5">
+        <v>104449</v>
+      </c>
+      <c r="D2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="E2" s="5">
+        <v>104449</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5">
-        <v>104449</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
-        <v>104449</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I2" s="5">
+        <v>110088</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="5">
-        <v>110088</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>315000</v>
+      </c>
+      <c r="O2" s="7">
+        <v>303800</v>
+      </c>
+      <c r="P2" s="7">
+        <v>303800</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="7">
-        <v>315000</v>
-      </c>
-      <c r="O3" s="7">
-        <v>303800</v>
-      </c>
-      <c r="P3" s="7">
-        <v>303800</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-      <c r="R3" s="6" t="s">
+      <c r="S2" s="5">
+        <v>122.32</v>
+      </c>
+      <c r="T2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="5">
-        <v>122.32</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" s="5">
+      <c r="U2" s="5">
         <v>1000</v>
       </c>
+    </row>
+    <row r="3" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="10"/>
     </row>
     <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8"/>
@@ -1739,7 +1725,7 @@
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -1749,20 +1735,20 @@
       <c r="L8" s="11"/>
       <c r="M8" s="10"/>
       <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
+      <c r="O8" s="10"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="11"/>
       <c r="S8" s="10"/>
       <c r="T8" s="11"/>
-      <c r="U8" s="10"/>
+      <c r="U8" s="11"/>
     </row>
     <row r="9" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -1772,13 +1758,13 @@
       <c r="L9" s="11"/>
       <c r="M9" s="10"/>
       <c r="N9" s="12"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="11"/>
       <c r="S9" s="10"/>
       <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
+      <c r="U9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8"/>
@@ -1801,7 +1787,7 @@
       <c r="R10" s="11"/>
       <c r="S10" s="10"/>
       <c r="T10" s="11"/>
-      <c r="U10" s="10"/>
+      <c r="U10" s="11"/>
     </row>
     <row r="11" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
@@ -1833,16 +1819,16 @@
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="11"/>
       <c r="I12" s="10"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="10"/>
       <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="12"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="11"/>
       <c r="S12" s="10"/>
@@ -1854,7 +1840,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="11"/>
@@ -1864,20 +1850,20 @@
       <c r="L13" s="13"/>
       <c r="M13" s="10"/>
       <c r="N13" s="12"/>
-      <c r="O13" s="10"/>
+      <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="11"/>
       <c r="S13" s="10"/>
       <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
+      <c r="U13" s="10"/>
     </row>
     <row r="14" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="11"/>
@@ -1887,20 +1873,20 @@
       <c r="L14" s="13"/>
       <c r="M14" s="10"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
+      <c r="O14" s="10"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="11"/>
       <c r="S14" s="10"/>
       <c r="T14" s="11"/>
-      <c r="U14" s="10"/>
+      <c r="U14" s="11"/>
     </row>
     <row r="15" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="11"/>
@@ -1910,27 +1896,27 @@
       <c r="L15" s="13"/>
       <c r="M15" s="10"/>
       <c r="N15" s="12"/>
-      <c r="O15" s="10"/>
+      <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="11"/>
       <c r="S15" s="10"/>
       <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
+      <c r="U15" s="10"/>
     </row>
     <row r="16" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="10"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="13"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="10"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
@@ -2038,7 +2024,7 @@
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2107,18 +2093,18 @@
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="10"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="10"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
+      <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="11"/>
       <c r="S24" s="10"/>
@@ -2138,10 +2124,10 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="12"/>
+      <c r="M25" s="10"/>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
-      <c r="P25" s="10"/>
+      <c r="P25" s="12"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="11"/>
       <c r="S25" s="10"/>
@@ -2160,7 +2146,7 @@
       <c r="I26" s="10"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
-      <c r="L26" s="13"/>
+      <c r="L26" s="11"/>
       <c r="M26" s="10"/>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
@@ -2199,7 +2185,7 @@
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="10"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -2222,7 +2208,7 @@
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -2255,20 +2241,20 @@
       <c r="L30" s="11"/>
       <c r="M30" s="10"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="12"/>
       <c r="R30" s="11"/>
       <c r="S30" s="10"/>
       <c r="T30" s="11"/>
-      <c r="U30" s="10"/>
+      <c r="U30" s="11"/>
     </row>
     <row r="31" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="10"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
@@ -2278,13 +2264,13 @@
       <c r="L31" s="11"/>
       <c r="M31" s="10"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="10"/>
       <c r="R31" s="11"/>
       <c r="S31" s="10"/>
       <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
+      <c r="U31" s="10"/>
     </row>
     <row r="32" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8"/>
@@ -2314,7 +2300,7 @@
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
@@ -2337,7 +2323,7 @@
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="10"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
@@ -2347,13 +2333,13 @@
       <c r="L34" s="11"/>
       <c r="M34" s="10"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
+      <c r="O34" s="10"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="11"/>
       <c r="S34" s="10"/>
       <c r="T34" s="11"/>
-      <c r="U34" s="10"/>
+      <c r="U34" s="11"/>
     </row>
     <row r="35" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="8"/>
@@ -2370,13 +2356,13 @@
       <c r="L35" s="11"/>
       <c r="M35" s="10"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="10"/>
+      <c r="O35" s="12"/>
       <c r="P35" s="12"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="11"/>
       <c r="S35" s="10"/>
       <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
+      <c r="U35" s="10"/>
     </row>
     <row r="36" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8"/>
@@ -2406,7 +2392,7 @@
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
@@ -2429,7 +2415,7 @@
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="E38" s="11"/>
       <c r="F38" s="10"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
@@ -2462,13 +2448,13 @@
       <c r="L39" s="11"/>
       <c r="M39" s="10"/>
       <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
+      <c r="O39" s="10"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="10"/>
       <c r="R39" s="11"/>
       <c r="S39" s="10"/>
       <c r="T39" s="11"/>
-      <c r="U39" s="10"/>
+      <c r="U39" s="11"/>
     </row>
     <row r="40" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8"/>
@@ -2485,13 +2471,13 @@
       <c r="L40" s="11"/>
       <c r="M40" s="10"/>
       <c r="N40" s="12"/>
-      <c r="O40" s="10"/>
+      <c r="O40" s="12"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="10"/>
       <c r="R40" s="11"/>
       <c r="S40" s="10"/>
       <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
+      <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="8"/>
@@ -2567,7 +2553,7 @@
       <c r="B44" s="9"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="11"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
@@ -2600,20 +2586,20 @@
       <c r="L45" s="11"/>
       <c r="M45" s="10"/>
       <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="12"/>
       <c r="R45" s="11"/>
       <c r="S45" s="10"/>
       <c r="T45" s="11"/>
-      <c r="U45" s="10"/>
+      <c r="U45" s="11"/>
     </row>
     <row r="46" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="10"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
@@ -2636,7 +2622,7 @@
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
+      <c r="E47" s="10"/>
       <c r="F47" s="10"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
@@ -2646,13 +2632,13 @@
       <c r="L47" s="11"/>
       <c r="M47" s="10"/>
       <c r="N47" s="12"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="10"/>
       <c r="R47" s="11"/>
       <c r="S47" s="10"/>
       <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
+      <c r="U47" s="10"/>
     </row>
     <row r="48" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="8"/>
@@ -2669,13 +2655,13 @@
       <c r="L48" s="11"/>
       <c r="M48" s="10"/>
       <c r="N48" s="12"/>
-      <c r="O48" s="12"/>
-      <c r="P48" s="12"/>
-      <c r="Q48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="12"/>
       <c r="R48" s="11"/>
       <c r="S48" s="10"/>
       <c r="T48" s="11"/>
-      <c r="U48" s="10"/>
+      <c r="U48" s="11"/>
     </row>
     <row r="49" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="8"/>
@@ -2723,33 +2709,7 @@
       <c r="T50" s="11"/>
       <c r="U50" s="11"/>
     </row>
-    <row r="51" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="8"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="10"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="12"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="10"/>
-      <c r="T51" s="11"/>
-      <c r="U51" s="11"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:U1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>